<commit_message>
Worked on evaluation for manuscript
Improved code, created new figures, added new statistics
</commit_message>
<xml_diff>
--- a/evaluation/BNC_ElanForumRig1.xlsx
+++ b/evaluation/BNC_ElanForumRig1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elen/Documents/PhD/Publications/2023_Shakir_LeFoll/MFTE_python/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1431F2C7-69F9-A148-B9DD-5B75F21F8EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F898BB4D-B500-EE41-A313-C81E9F29C2A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{99C2E5B7-8F9E-2340-9691-42D4291E387A}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4155" uniqueCount="1085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4156" uniqueCount="1086">
   <si>
     <t>WRAG_NN</t>
   </si>
@@ -3393,6 +3393,9 @@
   </si>
   <si>
     <t>NNMention</t>
+  </si>
+  <si>
+    <t>Tag4</t>
   </si>
 </sst>
 </file>
@@ -3782,10 +3785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DA7C31-E30C-674E-8A0E-5517363614C6}">
-  <dimension ref="A1:I1339"/>
+  <dimension ref="A1:J1339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A692" zoomScale="176" workbookViewId="0">
-      <selection activeCell="I694" sqref="I694"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="176" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3794,10 +3797,10 @@
     <col min="4" max="4" width="10.83203125" style="6"/>
     <col min="6" max="6" width="10.83203125" style="6"/>
     <col min="8" max="8" width="10.83203125" style="6"/>
-    <col min="9" max="9" width="40.5" style="5" customWidth="1"/>
+    <col min="10" max="10" width="40.5" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1057</v>
       </c>
@@ -3822,8 +3825,11 @@
       <c r="H1" s="4" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I1" s="3" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3834,7 +3840,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3845,7 +3851,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3856,7 +3862,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3870,7 +3876,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3881,7 +3887,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3894,11 +3900,11 @@
       <c r="D7" s="6" t="s">
         <v>1065</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>1067</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3909,7 +3915,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3920,7 +3926,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3931,7 +3937,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3942,7 +3948,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3953,7 +3959,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3964,7 +3970,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3978,7 +3984,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -3989,7 +3995,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -4182,7 +4188,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -4193,7 +4199,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -4204,7 +4210,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -4217,11 +4223,11 @@
       <c r="D35" s="6" t="s">
         <v>669</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="J35" s="5" t="s">
         <v>1066</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -4232,7 +4238,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -4243,7 +4249,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>28</v>
       </c>
@@ -4254,7 +4260,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -4265,7 +4271,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -4276,7 +4282,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -4287,7 +4293,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>32</v>
       </c>
@@ -4301,7 +4307,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -4314,11 +4320,11 @@
       <c r="D43" s="6" t="s">
         <v>567</v>
       </c>
-      <c r="I43" s="5" t="s">
+      <c r="J43" s="5" t="s">
         <v>1068</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -4329,7 +4335,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -4340,7 +4346,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -4351,7 +4357,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -4365,7 +4371,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -8571,7 +8577,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="417" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>236</v>
       </c>
@@ -8585,7 +8591,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="418" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>237</v>
       </c>
@@ -8596,7 +8602,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="419" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>238</v>
       </c>
@@ -8607,7 +8613,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="420" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>239</v>
       </c>
@@ -8621,7 +8627,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="421" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>28</v>
       </c>
@@ -8632,7 +8638,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="422" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>63</v>
       </c>
@@ -8643,7 +8649,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="423" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>240</v>
       </c>
@@ -8654,7 +8660,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="424" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>15</v>
       </c>
@@ -8665,7 +8671,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="425" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>241</v>
       </c>
@@ -8676,7 +8682,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="426" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
         <v>242</v>
       </c>
@@ -8687,7 +8693,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="427" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>243</v>
       </c>
@@ -8698,7 +8704,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="428" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>244</v>
       </c>
@@ -8708,11 +8714,11 @@
       <c r="C428" t="s">
         <v>554</v>
       </c>
-      <c r="I428" s="5" t="s">
+      <c r="J428" s="5" t="s">
         <v>1073</v>
       </c>
     </row>
-    <row r="429" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>245</v>
       </c>
@@ -8723,7 +8729,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="430" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>101</v>
       </c>
@@ -8734,7 +8740,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="431" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>28</v>
       </c>
@@ -8745,7 +8751,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="432" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
         <v>171</v>
       </c>
@@ -9302,7 +9308,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="481" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
         <v>266</v>
       </c>
@@ -9313,7 +9319,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="482" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
         <v>267</v>
       </c>
@@ -9324,7 +9330,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="483" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A483" t="s">
         <v>268</v>
       </c>
@@ -9335,7 +9341,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="484" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
         <v>269</v>
       </c>
@@ -9348,11 +9354,11 @@
       <c r="D484" s="6" t="s">
         <v>528</v>
       </c>
-      <c r="I484" s="5" t="s">
+      <c r="J484" s="5" t="s">
         <v>1071</v>
       </c>
     </row>
-    <row r="485" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A485" t="s">
         <v>6</v>
       </c>
@@ -9363,7 +9369,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="486" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A486" t="s">
         <v>270</v>
       </c>
@@ -9374,7 +9380,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="487" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A487" t="s">
         <v>71</v>
       </c>
@@ -9385,7 +9391,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="488" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A488" t="s">
         <v>57</v>
       </c>
@@ -9396,7 +9402,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="489" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A489" t="s">
         <v>169</v>
       </c>
@@ -9407,7 +9413,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="490" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A490" t="s">
         <v>271</v>
       </c>
@@ -9418,7 +9424,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="491" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
         <v>170</v>
       </c>
@@ -9429,7 +9435,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="492" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A492" t="s">
         <v>86</v>
       </c>
@@ -9440,7 +9446,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="493" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
         <v>272</v>
       </c>
@@ -9451,7 +9457,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="494" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
         <v>273</v>
       </c>
@@ -9462,7 +9468,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="495" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
         <v>35</v>
       </c>
@@ -9473,7 +9479,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="496" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
         <v>274</v>
       </c>
@@ -13301,7 +13307,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="833" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="833" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A833" t="s">
         <v>49</v>
       </c>
@@ -13312,7 +13318,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="834" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="834" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A834" t="s">
         <v>28</v>
       </c>
@@ -13323,7 +13329,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="835" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="835" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A835" t="s">
         <v>45</v>
       </c>
@@ -13334,7 +13340,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="836" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="836" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A836" t="s">
         <v>349</v>
       </c>
@@ -13345,7 +13351,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="837" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="837" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A837" t="s">
         <v>14</v>
       </c>
@@ -13356,7 +13362,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="838" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="838" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A838" t="s">
         <v>110</v>
       </c>
@@ -13367,7 +13373,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="839" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="839" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A839" t="s">
         <v>378</v>
       </c>
@@ -13378,7 +13384,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="840" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="840" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A840" t="s">
         <v>47</v>
       </c>
@@ -13389,7 +13395,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="841" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="841" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A841" t="s">
         <v>379</v>
       </c>
@@ -13400,7 +13406,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="842" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="842" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A842" t="s">
         <v>145</v>
       </c>
@@ -13411,7 +13417,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="843" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="843" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A843" t="s">
         <v>352</v>
       </c>
@@ -13425,7 +13431,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="844" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="844" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A844" t="s">
         <v>86</v>
       </c>
@@ -13436,7 +13442,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="845" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="845" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A845" t="s">
         <v>380</v>
       </c>
@@ -13446,11 +13452,11 @@
       <c r="C845" t="s">
         <v>931</v>
       </c>
-      <c r="I845" s="5" t="s">
+      <c r="J845" s="5" t="s">
         <v>1074</v>
       </c>
     </row>
-    <row r="846" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="846" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A846" t="s">
         <v>146</v>
       </c>
@@ -13461,7 +13467,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="847" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="847" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A847" t="s">
         <v>381</v>
       </c>
@@ -13472,7 +13478,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="848" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="848" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A848" t="s">
         <v>345</v>
       </c>
@@ -13665,7 +13671,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="865" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="865" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A865" t="s">
         <v>385</v>
       </c>
@@ -13675,11 +13681,11 @@
       <c r="C865" t="s">
         <v>567</v>
       </c>
-      <c r="I865" s="5" t="s">
+      <c r="J865" s="5" t="s">
         <v>1075</v>
       </c>
     </row>
-    <row r="866" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="866" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A866" t="s">
         <v>86</v>
       </c>
@@ -13690,7 +13696,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="867" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="867" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A867" t="s">
         <v>386</v>
       </c>
@@ -13704,7 +13710,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="868" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="868" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A868" t="s">
         <v>28</v>
       </c>
@@ -13715,7 +13721,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="869" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="869" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A869" t="s">
         <v>347</v>
       </c>
@@ -13726,7 +13732,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="870" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="870" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A870" t="s">
         <v>387</v>
       </c>
@@ -13737,7 +13743,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="871" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="871" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A871" t="s">
         <v>355</v>
       </c>
@@ -13748,7 +13754,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="872" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="872" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A872" t="s">
         <v>349</v>
       </c>
@@ -13759,7 +13765,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="873" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="873" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A873" t="s">
         <v>14</v>
       </c>
@@ -13770,7 +13776,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="874" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="874" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A874" t="s">
         <v>388</v>
       </c>
@@ -13781,7 +13787,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="875" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="875" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A875" t="s">
         <v>47</v>
       </c>
@@ -13792,7 +13798,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="876" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="876" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A876" t="s">
         <v>354</v>
       </c>
@@ -13803,7 +13809,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="877" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="877" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A877" t="s">
         <v>6</v>
       </c>
@@ -13814,7 +13820,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="878" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="878" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A878" t="s">
         <v>345</v>
       </c>
@@ -13825,7 +13831,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="879" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="879" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A879" t="s">
         <v>248</v>
       </c>
@@ -13839,7 +13845,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="880" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="880" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A880" t="s">
         <v>389</v>
       </c>

</xml_diff>